<commit_message>
simplified plus add sodium and fiber
</commit_message>
<xml_diff>
--- a/21_day_menu_database_wk3_tuesday_with_usda.xlsx
+++ b/21_day_menu_database_wk3_tuesday_with_usda.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\menu_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FFF049-CFB8-407F-BB99-90880E395B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3_Tues" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -193,11 +199,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,13 +267,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -305,7 +319,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -339,6 +353,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -373,9 +388,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,14 +564,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="17.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.9453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>45888</v>
       </c>
@@ -661,7 +683,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>45888</v>
       </c>
@@ -705,7 +727,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>45888</v>
       </c>
@@ -758,7 +780,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>45888</v>
       </c>
@@ -811,7 +833,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>45888</v>
       </c>
@@ -864,7 +886,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>45888</v>
       </c>
@@ -905,7 +927,7 @@
         <v>53</v>
       </c>
       <c r="R7">
-        <v>141.8</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="S7" t="s">
         <v>54</v>
@@ -914,7 +936,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>45888</v>
       </c>
@@ -943,7 +965,7 @@
         <v>210</v>
       </c>
       <c r="K8">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="L8">
         <v>6.4</v>
@@ -964,7 +986,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>45888</v>
       </c>
@@ -1014,7 +1036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>45888</v>
       </c>
@@ -1064,7 +1086,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>45888</v>
       </c>
@@ -1093,7 +1115,7 @@
         <v>5.03</v>
       </c>
       <c r="L11">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1111,7 +1133,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>45888</v>
       </c>
@@ -1164,7 +1186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>45888</v>
       </c>
@@ -1214,7 +1236,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>45888</v>
       </c>
@@ -1264,7 +1286,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>45888</v>
       </c>
@@ -1314,7 +1336,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>45888</v>
       </c>
@@ -1364,7 +1386,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>45888</v>
       </c>
@@ -1393,7 +1415,7 @@
         <v>70</v>
       </c>
       <c r="K17">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="L17">
         <v>6.36</v>
@@ -1414,7 +1436,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2">
         <v>45888</v>
       </c>
@@ -1443,7 +1465,7 @@
         <v>70</v>
       </c>
       <c r="K18">
-        <v>1.13</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="L18">
         <v>6.36</v>

</xml_diff>